<commit_message>
Added reverse calculations for thermistor
</commit_message>
<xml_diff>
--- a/Subsystems/Electronics/Sensors/Thermistor.xlsx
+++ b/Subsystems/Electronics/Sensors/Thermistor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\Resources\Subsystems\Electronics\Sensors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\CougsInSpace\Resources\Subsystems\Electronics\Sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50013346-3A8F-4469-A650-B5205D9CC8B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7B3754-57F6-41C2-9385-67ADDA4D087C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="3375" windowWidth="38700" windowHeight="15885" xr2:uid="{D0B171FA-B094-4AFC-9099-BFD1A498A54C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{D0B171FA-B094-4AFC-9099-BFD1A498A54C}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Beta</t>
   </si>
@@ -69,6 +69,21 @@
   <si>
     <t>Source Voltage</t>
   </si>
+  <si>
+    <t>Voltage Fraction</t>
+  </si>
+  <si>
+    <t>Fraction 298K</t>
+  </si>
+  <si>
+    <t>Fraction 333K</t>
+  </si>
+  <si>
+    <t>Resistance 298K</t>
+  </si>
+  <si>
+    <t>Resistance 333K</t>
+  </si>
 </sst>
 </file>
 
@@ -81,7 +96,7 @@
     <numFmt numFmtId="167" formatCode="0.0\ &quot;V&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00\ &quot;mW&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +122,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,14 +212,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -208,8 +232,16 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="4" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
@@ -3170,6 +3202,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1041058911"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -3184,6 +3217,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1041056831"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3837,7 +3871,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4165,18 +4199,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920B95C1-16DF-4844-B404-B15BB9463983}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4184,7 +4219,7 @@
         <v>3960</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
@@ -4192,7 +4227,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -4200,24 +4235,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="8">
         <f>B2*EXP(-B1*(1/(273.15+B3)-1/(273.15+B4)))</f>
-        <v>3578.8840959555769</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9153.0147876658357</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -4225,12 +4260,92 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="7">
         <v>3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="17">
+        <f>Data!C77</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="17">
+        <f>Data!C112</f>
+        <v>0.19855225068869667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="15">
+        <f>1/B11-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="16">
+        <f>1/B12-1</f>
+        <v>4.0364576404014985</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="15">
+        <f>LN(B14/B15)/(1/298-1/333)</f>
+        <v>-3956.2256306204067</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="14">
+        <f>(1/B19-1)/B14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="15">
+        <f>1/(1/298+LN(B20)/B17)-273</f>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4244,20 +4359,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33C94C4-B465-43AA-A0B7-9F4E84D37547}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" activeCellId="1" sqref="A1:A1048576 C1:E1048576"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4274,7 +4389,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>-50</v>
       </c>
@@ -4295,7 +4410,7 @@
         <v>1.2398296050143578E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>-49</v>
       </c>
@@ -4316,7 +4431,7 @@
         <v>1.3407192240680512E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>-48</v>
       </c>
@@ -4337,7 +4452,7 @@
         <v>1.4487024539834747E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>-47</v>
       </c>
@@ -4358,7 +4473,7 @@
         <v>1.5641860147673523E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>-46</v>
       </c>
@@ -4379,7 +4494,7 @@
         <v>1.6875926066942368E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>-45</v>
       </c>
@@ -4400,7 +4515,7 @@
         <v>1.8193609186837146E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>-44</v>
       </c>
@@ -4421,7 +4536,7 @@
         <v>1.9599455675094225E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>-43</v>
       </c>
@@ -4442,7 +4557,7 @@
         <v>2.1098169608740114E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>-42</v>
       </c>
@@ -4463,7 +4578,7 @@
         <v>2.2694610771265399E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>-41</v>
       </c>
@@ -4484,7 +4599,7 @@
         <v>2.4393791541784036E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>-40</v>
       </c>
@@ -4505,7 +4620,7 @@
         <v>2.6200872799994432E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>-39</v>
       </c>
@@ -4526,7 +4641,7 @@
         <v>2.8121158769570151E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>-38</v>
       </c>
@@ -4547,7 +4662,7 @@
         <v>3.0160090722075705E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>-37</v>
       </c>
@@ -4568,7 +4683,7 @@
         <v>3.2323239463739335E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>-36</v>
       </c>
@@ -4589,7 +4704,7 @@
         <v>3.4616296528530675E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>-35</v>
       </c>
@@ -4610,7 +4725,7 @@
         <v>3.7045064003112249E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>-34</v>
       </c>
@@ -4631,7 +4746,7 @@
         <v>3.9615442912476997E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>-33</v>
       </c>
@@ -4652,7 +4767,7 @@
         <v>4.2333420099577627E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>-32</v>
       </c>
@@ -4673,7 +4788,7 @@
         <v>4.5205053538114333E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>-31</v>
       </c>
@@ -4694,7 +4809,7 @@
         <v>4.8236456024999694E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>-30</v>
       </c>
@@ -4715,7 +4830,7 @@
         <v>5.1433777207964756E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>-29</v>
       </c>
@@ -4736,7 +4851,7 @@
         <v>5.480318391441337E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>-28</v>
       </c>
@@ -4757,7 +4872,7 @@
         <v>5.8350838760047569E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>-27</v>
       </c>
@@ -4778,7 +4893,7 @@
         <v>6.208287703003789E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>-26</v>
       </c>
@@ -4799,7 +4914,7 @@
         <v>6.600538184164137E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>-25</v>
       </c>
@@ -4820,7 +4935,7 @@
         <v>7.0124357615159102E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>-24</v>
       </c>
@@ -4841,7 +4956,7 @@
         <v>7.4445701899970046E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>-23</v>
       </c>
@@ -4862,7 +4977,7 @@
         <v>7.8975175623972577E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>-22</v>
       </c>
@@ -4883,7 +4998,7 @@
         <v>8.3718371858020585E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>-21</v>
       </c>
@@ -4904,7 +5019,7 @@
         <v>8.8680683211644282E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>-20</v>
       </c>
@@ -4925,7 +5040,7 @@
         <v>9.3867268002317511E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>-19</v>
       </c>
@@ -4946,7 +5061,7 @@
         <v>9.9283015367428437E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>-18</v>
       </c>
@@ -4967,7 +5082,7 @@
         <v>0.10493250951564162</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>-17</v>
       </c>
@@ -4988,7 +5103,7 @@
         <v>0.11081999334204733</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>-16</v>
       </c>
@@ -5009,7 +5124,7 @@
         <v>0.11694933165895212</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>-15</v>
       </c>
@@ -5030,7 +5145,7 @@
         <v>0.12332397432082959</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>-14</v>
       </c>
@@ -5051,7 +5166,7 @@
         <v>0.12994691954726503</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>-13</v>
       </c>
@@ -5072,7 +5187,7 @@
         <v>0.13682067777108139</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>-12</v>
       </c>
@@ -5093,7 +5208,7 @@
         <v>0.14394723635958637</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>-11</v>
       </c>
@@ -5114,7 +5229,7 @@
         <v>0.15132802557438987</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>-10</v>
       </c>
@@ -5135,7 +5250,7 @@
         <v>0.15896388614883891</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>-9</v>
       </c>
@@ -5156,7 +5271,7 @@
         <v>0.16685503887119149</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>-8</v>
       </c>
@@ -5177,7 +5292,7 @@
         <v>0.17500105656558204</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>-7</v>
       </c>
@@ -5198,7 +5313,7 @@
         <v>0.1834008388611173</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>-6</v>
       </c>
@@ -5219,7 +5334,7 @@
         <v>0.19205259013158485</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>-5</v>
       </c>
@@ -5240,7 +5355,7 @@
         <v>0.20095380097395293</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>-4</v>
       </c>
@@ -5261,7 +5376,7 @@
         <v>0.21010123357281887</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>-3</v>
       </c>
@@ -5282,7 +5397,7 @@
         <v>0.2194909112701571</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>-2</v>
       </c>
@@ -5303,7 +5418,7 @@
         <v>0.22911811262518811</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>-1</v>
       </c>
@@ -5324,7 +5439,7 @@
         <v>0.23897737020816978</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>0</v>
       </c>
@@ -5345,7 +5460,7 @@
         <v>0.24906247432480072</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -5366,7 +5481,7 @@
         <v>0.2593664818153234</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -5387,7 +5502,7 @@
         <v>0.26988173001504678</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -5408,7 +5523,7 @@
         <v>0.2805998559018138</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>4</v>
       </c>
@@ -5429,7 +5544,7 @@
         <v>0.29151182039195411</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>5</v>
       </c>
@@ -5450,7 +5565,7 @@
         <v>0.30260793768065058</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>6</v>
       </c>
@@ -5471,7 +5586,7 @@
         <v>0.31387790945670346</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>7</v>
       </c>
@@ -5492,7 +5607,7 @@
         <v>0.32531086375667556</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>8</v>
       </c>
@@ -5513,7 +5628,7 @@
         <v>0.33689539816071989</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>9</v>
       </c>
@@ -5534,7 +5649,7 @@
         <v>0.34861962697330973</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>10</v>
       </c>
@@ -5555,7 +5670,7 @@
         <v>0.36047123197791342</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>11</v>
       </c>
@@ -5576,7 +5691,7 @@
         <v>0.37243751630650967</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>12</v>
       </c>
@@ -5597,7 +5712,7 @@
         <v>0.38450546092375021</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>13</v>
       </c>
@@ -5618,7 +5733,7 @@
         <v>0.39666178319246553</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>14</v>
       </c>
@@ -5639,7 +5754,7 @@
         <v>0.40889299696265347</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>15</v>
       </c>
@@ -5660,7 +5775,7 @@
         <v>0.42118547361065506</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>16</v>
       </c>
@@ -5681,7 +5796,7 @@
         <v>0.43352550344905383</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>17</v>
       </c>
@@ -5702,7 +5817,7 @@
         <v>0.44589935693099708</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>18</v>
       </c>
@@ -5723,7 +5838,7 @@
         <v>0.45829334508490038</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>19</v>
       </c>
@@ -5744,7 +5859,7 @@
         <v>0.47069387863639917</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>20</v>
       </c>
@@ -5765,7 +5880,7 @@
         <v>0.48308752530336152</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>21</v>
       </c>
@@ -5786,7 +5901,7 @@
         <v>0.49546106478595059</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>22</v>
       </c>
@@ -5807,7 +5922,7 @@
         <v>0.50780154101616226</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>23</v>
       </c>
@@ -5828,7 +5943,7 @@
         <v>0.52009631127894485</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>24</v>
       </c>
@@ -5849,7 +5964,7 @@
         <v>0.53233309186874567</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>25</v>
       </c>
@@ -5870,7 +5985,7 @@
         <v>0.54449999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>26</v>
       </c>
@@ -5891,7 +6006,7 @@
         <v>0.55658559174644928</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>27</v>
       </c>
@@ -5899,7 +6014,7 @@
         <f>Information!$B$2*EXP(-Information!$B$1*(1/(273.15+Information!$B$3)-1/(273.15+Data!A79)))</f>
         <v>9153.0147876658357</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="12">
         <f>B79/(B79+Information!$B$6)</f>
         <v>0.47788898453522816</v>
       </c>
@@ -5912,7 +6027,7 @@
         <v>0.5685788958411363</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>28</v>
       </c>
@@ -5933,7 +6048,7 @@
         <v>0.5804694432253561</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>29</v>
       </c>
@@ -5954,7 +6069,7 @@
         <v>0.59224729228970574</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>30</v>
       </c>
@@ -5975,7 +6090,7 @@
         <v>0.60390304980283815</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>31</v>
       </c>
@@ -5996,7 +6111,7 @@
         <v>0.61542788757269096</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>32</v>
       </c>
@@ -6017,7 +6132,7 @@
         <v>0.62681355493025959</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>33</v>
       </c>
@@ -6038,7 +6153,7 @@
         <v>0.63805238716686719</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>34</v>
       </c>
@@ -6059,7 +6174,7 @@
         <v>0.64913731009195152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>35</v>
       </c>
@@ -6080,7 +6195,7 @@
         <v>0.66006184090940989</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>36</v>
       </c>
@@ -6101,7 +6216,7 @@
         <v>0.67082008563644735</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>37</v>
       </c>
@@ -6122,7 +6237,7 @@
         <v>0.68140673330955748</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>38</v>
       </c>
@@ -6143,7 +6258,7 @@
         <v>0.69181704723797655</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>39</v>
       </c>
@@ -6164,7 +6279,7 @@
         <v>0.70204685357577068</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>40</v>
       </c>
@@ -6185,7 +6300,7 @@
         <v>0.71209252749000451</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>41</v>
       </c>
@@ -6206,7 +6321,7 @@
         <v>0.72195097720451085</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>42</v>
       </c>
@@ -6227,7 +6342,7 @@
         <v>0.73161962619701959</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>43</v>
       </c>
@@ -6248,7 +6363,7 @@
         <v>0.74109639382224157</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>44</v>
       </c>
@@ -6269,7 +6384,7 @@
         <v>0.75037967462538135</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>45</v>
       </c>
@@ -6290,7 +6405,7 @@
         <v>0.75946831659990799</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>46</v>
       </c>
@@ -6311,7 +6426,7 @@
         <v>0.76836159863068698</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>47</v>
       </c>
@@ -6332,7 +6447,7 @@
         <v>0.77705920734920519</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>48</v>
       </c>
@@ -6353,7 +6468,7 @@
         <v>0.78556121361199138</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>49</v>
       </c>
@@ -6374,7 +6489,7 @@
         <v>0.79386804879684114</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>50</v>
       </c>
@@ -6395,7 +6510,7 @@
         <v>0.8019804810944331</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>51</v>
       </c>
@@ -6416,7 +6531,7 @@
         <v>0.80989959195566985</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>52</v>
       </c>
@@ -6437,7 +6552,7 @@
         <v>0.81762675283790343</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>53</v>
       </c>
@@ -6458,7 +6573,7 @@
         <v>0.82516360237628927</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>54</v>
       </c>
@@ -6479,7 +6594,7 @@
         <v>0.83251202409011882</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>55</v>
       </c>
@@ -6500,7 +6615,7 @@
         <v>0.83967412471821468</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>56</v>
       </c>
@@ -6521,7 +6636,7 @@
         <v>0.84665221326250995</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>57</v>
       </c>
@@ -6542,7 +6657,7 @@
         <v>0.85344878080483944</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>58</v>
       </c>
@@ -6563,7 +6678,7 @@
         <v>0.8600664811488512</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>59</v>
       </c>
@@ -6584,7 +6699,7 @@
         <v>0.86650811232681413</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>60</v>
       </c>
@@ -6605,7 +6720,7 @@
         <v>0.87277659900000915</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>61</v>
       </c>
@@ -6626,7 +6741,7 @@
         <v>0.8788749757713179</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>62</v>
       </c>
@@ -6647,7 +6762,7 @@
         <v>0.88480637141958929</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>63</v>
       </c>
@@ -6668,7 +6783,7 @@
         <v>0.89057399405731807</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>64</v>
       </c>
@@ -6689,7 +6804,7 @@
         <v>0.89618111720608351</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>65</v>
       </c>
@@ -6710,7 +6825,7 @@
         <v>0.90163106677802629</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>66</v>
       </c>
@@ -6731,7 +6846,7 @@
         <v>0.90692720894635015</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>67</v>
       </c>
@@ -6739,7 +6854,7 @@
         <f>Information!$B$2*EXP(-Information!$B$1*(1/(273.15+Information!$B$3)-1/(273.15+Data!A119)))</f>
         <v>1939.8345633770634</v>
       </c>
-      <c r="C119" s="3">
+      <c r="C119" s="12">
         <f>B119/(B119+Information!$B$6)</f>
         <v>0.16246745740741658</v>
       </c>
@@ -6752,7 +6867,7 @@
         <v>0.91207293888332319</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120" s="2">
         <v>68</v>
       </c>
@@ -6773,7 +6888,7 @@
         <v>0.91707167034052917</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121" s="2">
         <v>69</v>
       </c>
@@ -6794,7 +6909,7 @@
         <v>0.92192682604304743</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122" s="2">
         <v>70</v>
       </c>
@@ -6815,7 +6930,7 @@
         <v>0.92664182886683133</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A123" s="2">
         <v>71</v>
       </c>
@@ -6836,7 +6951,7 @@
         <v>0.9312200937666848</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A124" s="2">
         <v>72</v>
       </c>
@@ -6857,7 +6972,7 @@
         <v>0.93566502042090294</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A125" s="2">
         <v>73</v>
       </c>
@@ -6878,7 +6993,7 @@
         <v>0.93997998655774395</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A126" s="2">
         <v>74</v>
       </c>
@@ -6899,7 +7014,7 @@
         <v>0.94416834192841814</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A127" s="2">
         <v>75</v>
       </c>
@@ -6920,7 +7035,7 @@
         <v>0.94823340289112845</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A128" s="2">
         <v>76</v>
       </c>
@@ -6941,7 +7056,7 @@
         <v>0.95217844757087911</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A129" s="2">
         <v>77</v>
       </c>
@@ -6962,7 +7077,7 @@
         <v>0.95600671156017114</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A130" s="2">
         <v>78</v>
       </c>
@@ -6983,7 +7098,7 @@
         <v>0.95972138412637076</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131" s="2">
         <v>79</v>
       </c>
@@ -7004,7 +7119,7 @@
         <v>0.96332560489233932</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A132" s="2">
         <v>80</v>
       </c>
@@ -7025,7 +7140,7 @@
         <v>0.96682246095791069</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A133" s="2">
         <v>81</v>
       </c>
@@ -7046,7 +7161,7 @@
         <v>0.97021498443087939</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A134" s="2">
         <v>82</v>
       </c>
@@ -7067,7 +7182,7 @@
         <v>0.97350615033736676</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A135" s="2">
         <v>83</v>
       </c>
@@ -7088,7 +7203,7 @@
         <v>0.97669887488267604</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A136" s="2">
         <v>84</v>
       </c>
@@ -7109,7 +7224,7 @@
         <v>0.97979601403506633</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A137" s="2">
         <v>85</v>
       </c>
@@ -7130,7 +7245,7 @@
         <v>0.98280036240619972</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A138" s="2">
         <v>86</v>
       </c>
@@ -7151,7 +7266,7 @@
         <v>0.98571465240337586</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A139" s="2">
         <v>87</v>
       </c>
@@ -7172,7 +7287,7 @@
         <v>0.98854155363001461</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A140" s="2">
         <v>88</v>
       </c>
@@ -7193,7 +7308,7 @@
         <v>0.9912836725121863</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A141" s="2">
         <v>89</v>
       </c>
@@ -7214,7 +7329,7 @@
         <v>0.99394355213031793</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A142" s="2">
         <v>90</v>
       </c>

</xml_diff>